<commit_message>
Added Talent Hunt user.
</commit_message>
<xml_diff>
--- a/project/oneup/testdata/TestData.xlsx
+++ b/project/oneup/testdata/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\workspace\oneup\project\oneup\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SM_Automation\OneUp-Web-QA-master\OneUp-Web-QA-master\project\oneup\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7157709-A83C-4666-8FE5-36ECDD868BE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B883B689-A985-425F-93F4-83E4AB01A5A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="auto_projects" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
   <si>
     <t>projectid</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>amruta.bisain1+10@gmail.com</t>
+  </si>
+  <si>
+    <t>ONEUP_TALENTHUNT_USER</t>
+  </si>
+  <si>
+    <t>samruddhi.ubhad+th1@jiem.in</t>
   </si>
 </sst>
 </file>
@@ -231,11 +237,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -523,16 +530,16 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>14</v>
       </c>
@@ -576,17 +583,17 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -606,7 +613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -626,7 +633,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -653,26 +660,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35407932-E8FE-45A4-ADE9-AC545BEF6A08}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -701,7 +708,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -721,7 +728,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -741,7 +748,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -761,7 +768,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -781,7 +788,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -801,7 +808,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -821,7 +828,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -841,7 +848,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -861,7 +868,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -878,6 +885,66 @@
         <v>49</v>
       </c>
       <c r="I10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11">
+        <v>123456</v>
+      </c>
+      <c r="I11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12">
+        <v>123456</v>
+      </c>
+      <c r="I12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13">
+        <v>123456</v>
+      </c>
+      <c r="I13" t="s">
         <v>33</v>
       </c>
     </row>
@@ -887,6 +954,9 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{37D654D6-6157-4FA7-A4A0-D971FF039D4D}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{7F823308-0829-42F0-B9D7-16E70A107A55}"/>
     <hyperlink ref="D8" r:id="rId4" xr:uid="{79270087-D424-482F-8047-A1C78D91046B}"/>
+    <hyperlink ref="D11" r:id="rId5" xr:uid="{25ADD08B-A93F-427A-9773-1B845F2CBBD2}"/>
+    <hyperlink ref="D12" r:id="rId6" xr:uid="{A6D3952E-07B2-4CF8-A31B-7AE2C8EFF9D4}"/>
+    <hyperlink ref="D13" r:id="rId7" xr:uid="{731944E8-6504-4232-8CF0-E9551534D1B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -900,20 +970,20 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="71.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="6" max="6" width="71.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -942,7 +1012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -968,7 +1038,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -994,7 +1064,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>

</xml_diff>